<commit_message>
Updated Serial Number Upload - New UI - Improved Performance
</commit_message>
<xml_diff>
--- a/excel sheets/DUX Serial No (DUXNZ-2011-102-CN).xlsx
+++ b/excel sheets/DUX Serial No (DUXNZ-2011-102-CN).xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uberoisa\source\repos\serialnumberupload_bit\excel sheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6C1957-B734-4DDD-9050-157B82116E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="4035" windowWidth="20730" windowHeight="4050"/>
+    <workbookView xWindow="-25252" yWindow="-6755" windowWidth="25370" windowHeight="13667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FOR DUX" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FOR DUX'!$A$1:$G$7215</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FOR DUX'!$A$1:$G$7213</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="315">
   <si>
     <t>SERIAL NO.</t>
     <phoneticPr fontId="1"/>
@@ -85,12 +91,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>NF-1320201102002</t>
-  </si>
-  <si>
-    <t>NF-1320201102003</t>
-  </si>
-  <si>
     <t>NF-1320201102004</t>
   </si>
   <si>
@@ -980,18 +980,15 @@
   </si>
   <si>
     <t>NF-2520201102022</t>
-  </si>
-  <si>
-    <t>NF-2520201102023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="yyyymmdd"/>
-    <numFmt numFmtId="177" formatCode="0000000"/>
+    <numFmt numFmtId="164" formatCode="yyyymmdd"/>
+    <numFmt numFmtId="165" formatCode="0000000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -1057,7 +1054,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
@@ -1072,12 +1069,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1087,6 +1084,14 @@
       <color rgb="FF66FFCC"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1345,31 +1350,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G301"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G299"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.1"/>
   <cols>
-    <col min="1" max="1" width="10.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -2387,18 +2392,18 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B45" s="2">
-        <v>800339</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>9</v>
+        <v>800343</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D45" s="1">
         <v>1</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" s="4" t="s">
         <v>61</v>
       </c>
       <c r="F45" s="1" t="s">
@@ -2410,18 +2415,18 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B46" s="2">
-        <v>800339</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>9</v>
+        <v>800343</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D46" s="1">
         <v>1</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" s="4" t="s">
         <v>62</v>
       </c>
       <c r="F46" s="1" t="s">
@@ -2847,13 +2852,13 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B65" s="2">
-        <v>800343</v>
+        <v>800344</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D65" s="1">
         <v>1</v>
@@ -2870,13 +2875,13 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B66" s="2">
-        <v>800343</v>
+        <v>800344</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D66" s="1">
         <v>1</v>
@@ -3997,18 +4002,18 @@
     </row>
     <row r="115" spans="1:7">
       <c r="A115" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B115" s="2">
-        <v>800344</v>
+        <v>800347</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D115" s="1">
         <v>1</v>
       </c>
-      <c r="E115" s="4" t="s">
+      <c r="E115" s="1" t="s">
         <v>131</v>
       </c>
       <c r="F115" s="1" t="s">
@@ -4020,18 +4025,18 @@
     </row>
     <row r="116" spans="1:7">
       <c r="A116" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B116" s="2">
-        <v>800344</v>
+        <v>800347</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D116" s="1">
         <v>1</v>
       </c>
-      <c r="E116" s="4" t="s">
+      <c r="E116" s="1" t="s">
         <v>132</v>
       </c>
       <c r="F116" s="1" t="s">
@@ -6361,7 +6366,7 @@
         <v>17</v>
       </c>
       <c r="G217" s="1">
-        <v>201111</v>
+        <v>201112</v>
       </c>
     </row>
     <row r="218" spans="1:7">
@@ -6384,7 +6389,7 @@
         <v>17</v>
       </c>
       <c r="G218" s="1">
-        <v>201111</v>
+        <v>201112</v>
       </c>
     </row>
     <row r="219" spans="1:7">
@@ -7447,18 +7452,18 @@
     </row>
     <row r="265" spans="1:7">
       <c r="A265" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B265" s="2">
-        <v>800347</v>
+        <v>800348</v>
       </c>
       <c r="C265" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D265" s="1">
         <v>1</v>
       </c>
-      <c r="E265" s="1" t="s">
+      <c r="E265" s="4" t="s">
         <v>281</v>
       </c>
       <c r="F265" s="1" t="s">
@@ -7470,18 +7475,18 @@
     </row>
     <row r="266" spans="1:7">
       <c r="A266" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B266" s="2">
-        <v>800347</v>
+        <v>800348</v>
       </c>
       <c r="C266" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D266" s="1">
         <v>1</v>
       </c>
-      <c r="E266" s="1" t="s">
+      <c r="E266" s="4" t="s">
         <v>282</v>
       </c>
       <c r="F266" s="1" t="s">
@@ -8228,80 +8233,13 @@
       </c>
     </row>
     <row r="299" spans="1:7">
-      <c r="A299" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B299" s="2">
-        <v>800348</v>
-      </c>
-      <c r="C299" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D299" s="1">
-        <v>1</v>
-      </c>
-      <c r="E299" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="F299" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G299" s="1">
-        <v>201112</v>
-      </c>
-    </row>
-    <row r="300" spans="1:7">
-      <c r="A300" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B300" s="2">
-        <v>800348</v>
-      </c>
-      <c r="C300" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D300" s="1">
-        <v>1</v>
-      </c>
-      <c r="E300" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="F300" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G300" s="1">
-        <v>201112</v>
-      </c>
-    </row>
-    <row r="301" spans="1:7">
-      <c r="A301" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B301" s="2">
-        <v>800348</v>
-      </c>
-      <c r="C301" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D301" s="1">
-        <v>1</v>
-      </c>
-      <c r="E301" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="F301" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G301" s="1">
-        <v>201112</v>
-      </c>
+      <c r="B299" s="2"/>
+      <c r="C299" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G7215">
-    <filterColumn colId="1"/>
-  </autoFilter>
-  <sortState ref="A2:G625">
-    <sortCondition ref="B2:B625"/>
+  <autoFilter ref="A1:G7213" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G623">
+    <sortCondition ref="B2:B623"/>
   </sortState>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51200000000000001" footer="0.51200000000000001"/>

</xml_diff>